<commit_message>
Cam test file rearrangements
</commit_message>
<xml_diff>
--- a/cam_test/cam_tests (Autosaved).xlsx
+++ b/cam_test/cam_tests (Autosaved).xlsx
@@ -15,7 +15,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -604,7 +603,7 @@
   <dimension ref="A1:AU132"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AL1" workbookViewId="0">
-      <selection activeCell="AN3" sqref="AN3"/>
+      <selection activeCell="AT7" sqref="AT7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" thickTop="1" thickBottom="1" x14ac:dyDescent="0.3"/>
@@ -942,6 +941,12 @@
       <c r="U5" s="6"/>
       <c r="X5" s="6"/>
       <c r="Y5" s="6"/>
+      <c r="AN5" s="6"/>
+      <c r="AO5" s="6"/>
+      <c r="AP5" s="6"/>
+      <c r="AQ5" s="6"/>
+      <c r="AT5" s="6"/>
+      <c r="AU5" s="6"/>
     </row>
     <row r="6" spans="1:47" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
@@ -965,6 +970,14 @@
       <c r="AK6" s="6"/>
       <c r="AL6" s="6"/>
       <c r="AM6" s="6"/>
+      <c r="AN6" s="6"/>
+      <c r="AO6" s="6"/>
+      <c r="AP6" s="6"/>
+      <c r="AQ6" s="6"/>
+      <c r="AR6" s="6"/>
+      <c r="AS6" s="6"/>
+      <c r="AT6" s="6"/>
+      <c r="AU6" s="6"/>
     </row>
     <row r="7" spans="1:47" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
@@ -2360,6 +2373,16 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="V1:W1"/>
+    <mergeCell ref="X1:Y1"/>
+    <mergeCell ref="Z1:AA1"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="J1:K1"/>
     <mergeCell ref="AN1:AO1"/>
     <mergeCell ref="AP1:AQ1"/>
     <mergeCell ref="AR1:AS1"/>
@@ -2367,16 +2390,6 @@
     <mergeCell ref="N1:O1"/>
     <mergeCell ref="P1:Q1"/>
     <mergeCell ref="R1:S1"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="L1:M1"/>
-    <mergeCell ref="T1:U1"/>
-    <mergeCell ref="V1:W1"/>
-    <mergeCell ref="X1:Y1"/>
-    <mergeCell ref="Z1:AA1"/>
     <mergeCell ref="AB1:AC1"/>
     <mergeCell ref="AD1:AE1"/>
     <mergeCell ref="AF1:AG1"/>

</xml_diff>